<commit_message>
fixing grid, photo, random kode soal, etc
</commit_message>
<xml_diff>
--- a/Nilai Ujian KDS002.xlsx
+++ b/Nilai Ujian KDS002.xlsx
@@ -48,6 +48,9 @@
 Adanya perubahan kata ganti orang</t>
   </si>
   <si>
+    <t>Permata Aura</t>
+  </si>
+  <si>
     <t>Sebutkan apa saja ciri-ciri pantun!</t>
   </si>
   <si>
@@ -56,6 +59,11 @@
 Setiap baris memiliki rima akhir a-b-a-b</t>
   </si>
   <si>
+    <t>Setiap baris memiliki rima akhir a-b-a-b_x000D_
+Sampiran terdapat pada baris pertama dan kedua_x000D_
+Isi terdapat pada baris ketiga dan keempat</t>
+  </si>
+  <si>
     <t>Sebutkan apa saja ciri-ciri gurindam!</t>
   </si>
   <si>
@@ -64,39 +72,31 @@
 Rima pada tiap baris bersajak a-a, b-b, c-c, dan seterusnya</t>
   </si>
   <si>
+    <t>Soal, masalah, atau perjanjian terdapat pada baris pertama_x000D_
+Jawaban atau akibat terdapat pada baris kedua_x000D_
+Berisi tentang nasihat, kata-kata mutiara atau filosofi hidup</t>
+  </si>
+  <si>
     <t>Sebutkan unsur-unsur yang terdapat pada Fabel dan jelaskan!</t>
   </si>
   <si>
     <t>Tokoh; binatang menjadi pelaku dalam cerita baik tokoh protagonis maupun antagonis, tokoh utama (sering dibicarakan, sering muncul) atau pembantu (tambahan)_x000D_
 Penokohan dan watak tokoh; tokoh diberikan karakter atau sifat_x000D_
 setting, tema, amanat</t>
-  </si>
-  <si>
-    <t>Perbaikilah penggunaan huruf kapital pada teks berikut!_x000D_
-_x000D_
-gedong gincu diresmikan sebagai salah satu simbol indramayu. Peresmiannya dilakukan oleh ibu hj. anasophana pada puncak peringatan hari jadi indramayu yang ke-491, tanggal 7 oktober 2018.</t>
-  </si>
-  <si>
-    <t>Gedong gincu diresmikan sebagai salah 1 simbol Indramayu. Peresmiannya dilakukan oleh Ibu Hj. Ana Sophana pada puncak peringatan hari jadi Indramayu yang ke-491 tanggal 7 Oktober 2018.</t>
-  </si>
-  <si>
-    <t>Permata Aura</t>
-  </si>
-  <si>
-    <t>Setiap baris memiliki rima akhir a-b-a-b_x000D_
-Sampiran terdapat pada baris pertama dan kedua_x000D_
-Isi terdapat pada baris ketiga dan keempat</t>
-  </si>
-  <si>
-    <t>Soal, masalah, atau perjanjian terdapat pada baris pertama_x000D_
-Jawaban atau akibat terdapat pada baris kedua_x000D_
-Berisi tentang nasihat, kata-kata mutiara atau filosofi hidup</t>
   </si>
   <si>
     <t>Penokohan dan watak tokoh; tokoh diberikan karakter atau sifat_x000D_
 Setting/latar; tempat, waktu, sosial pada cerita_x000D_
 Tema; ide atau gagasan yang mendasari cerita_x000D_
 Amanat; pesan cerita tersebut</t>
+  </si>
+  <si>
+    <t>Perbaikilah penggunaan huruf kapital pada teks berikut!_x000D_
+_x000D_
+gedong gincu diresmikan sebagai salah satu simbol indramayu. Peresmiannya dilakukan oleh ibu hj. anasophana pada puncak peringatan hari jadi indramayu yang ke-491, tanggal 7 oktober 2018.</t>
+  </si>
+  <si>
+    <t>Gedong gincu diresmikan sebagai salah 1 simbol Indramayu. Peresmiannya dilakukan oleh Ibu Hj. Ana Sophana pada puncak peringatan hari jadi Indramayu yang ke-491 tanggal 7 Oktober 2018.</t>
   </si>
   <si>
     <t>Gedong Gincu diresmikan sebagai salah satu symbol Indramayu. Peresmiannya dilakukan oleh Ibu Hj. Ana Sophana pada puncak peringatan hari jadi Indramayu yang ke-491 tanggal 7 Oktober 2018.</t>
@@ -482,19 +482,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F3">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -508,13 +508,13 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
       <c r="F4">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -522,19 +522,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5">
         <v>14</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -548,13 +548,13 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F6">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -562,19 +562,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="F7">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -582,19 +582,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
       <c r="F8">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -602,19 +602,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -622,19 +622,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -642,13 +642,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
         <v>22</v>

</xml_diff>